<commit_message>
fix left hand and right hand
</commit_message>
<xml_diff>
--- a/diagram/left_hand_diagram.xlsx
+++ b/diagram/left_hand_diagram.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Agiat_Ikazinat\Agiat_Ikazinat\diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB537603-0472-4E9E-989A-67B55F0258C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFB82DB2-CFB2-4975-AF33-13C041E89784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880" xr2:uid="{8CF7E09D-69CB-4638-9570-7402B5B5296D}"/>
+    <workbookView xWindow="2448" yWindow="1092" windowWidth="17280" windowHeight="8880" xr2:uid="{8CF7E09D-69CB-4638-9570-7402B5B5296D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>Name</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>open</t>
+  </si>
+  <si>
+    <t>rotate_inside</t>
+  </si>
+  <si>
+    <t>rotate_outside</t>
   </si>
 </sst>
 </file>
@@ -467,7 +473,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -500,7 +506,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -520,7 +526,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -540,7 +546,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -560,7 +566,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -580,7 +586,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -600,7 +606,19 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7">
+        <v>180</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>